<commit_message>
modified:   src/main/java/org/example/Cart.xlsx 	modified:   src/main/java/org/example/Client.xlsx 	modified:   src/main/java/org/example/ClientPasswordManage.java 	modified:   src/main/java/org/example/ExcelIn.java 	modified:   src/main/java/org/example/Goods.xlsx 	modified:   src/main/java/org/example/History.xlsx 	modified:   src/main/java/org/example/ModifyPassword.java 	modified:   src/main/java/org/example/Users.xlsx
</commit_message>
<xml_diff>
--- a/src/main/java/org/example/Goods.xlsx
+++ b/src/main/java/org/example/Goods.xlsx
@@ -41,16 +41,16 @@
     <t>雷蛇</t>
   </si>
   <si>
-    <t>鼠标</t>
-  </si>
-  <si>
-    <t>罗技</t>
-  </si>
-  <si>
     <t>水杯</t>
   </si>
   <si>
     <t>青鸟</t>
+  </si>
+  <si>
+    <t>抽纸</t>
+  </si>
+  <si>
+    <t>清风</t>
   </si>
 </sst>
 </file>
@@ -132,7 +132,7 @@
         <v>589.0</v>
       </c>
       <c r="E2" t="n">
-        <v>99.0</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="3">
@@ -146,15 +146,15 @@
         <v>8</v>
       </c>
       <c r="D3" t="n">
-        <v>299.0</v>
+        <v>199.0</v>
       </c>
       <c r="E3" t="n">
-        <v>100.0</v>
+        <v>97.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -163,7 +163,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>69.0</v>
+        <v>25.0</v>
       </c>
       <c r="E4" t="n">
         <v>50.0</v>
@@ -171,7 +171,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -180,10 +180,10 @@
         <v>12</v>
       </c>
       <c r="D5" t="n">
-        <v>25.0</v>
+        <v>5.0</v>
       </c>
       <c r="E5" t="n">
-        <v>50.0</v>
+        <v>200.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>